<commit_message>
Tweede Kamerverkiezingen mobiel partij klikken
</commit_message>
<xml_diff>
--- a/doc/tk.xlsx
+++ b/doc/tk.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="77">
   <si>
     <t>      Naam partij      </t>
   </si>
@@ -367,7 +367,16 @@
     <t>BBB</t>
   </si>
   <si>
-    <t>Exitpol</t>
+    <t>Bij1</t>
+  </si>
+  <si>
+    <t>50plus</t>
+  </si>
+  <si>
+    <t>Denk</t>
+  </si>
+  <si>
+    <t>exitpol</t>
   </si>
 </sst>
 </file>
@@ -485,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -518,6 +527,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9532,10 +9542,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9555,7 +9565,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>60</v>
@@ -9563,31 +9573,31 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -9595,15 +9605,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>66</v>
@@ -9611,7 +9621,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -9619,10 +9629,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -9635,23 +9645,23 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>70</v>
@@ -9659,10 +9669,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -9673,8 +9683,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
         <v>73</v>
       </c>
     </row>
@@ -9697,110 +9710,110 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C23" t="str">
         <f>C22&amp;"&amp;"&amp;B23&amp;"="&amp;A23</f>
-        <v>VVD=35&amp;PVV=19</v>
+        <v>VVD=35&amp;D66=27</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" ref="C24:C37" si="0">C23&amp;"&amp;"&amp;B24&amp;"="&amp;A24</f>
-        <v>VVD=35&amp;PVV=19&amp;D66=18</v>
+        <f t="shared" ref="C24:C38" si="0">C23&amp;"&amp;"&amp;B24&amp;"="&amp;A24</f>
+        <v>VVD=35&amp;D66=27&amp;PVV=17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10&amp;CU=6</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
         <v>61</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10&amp;CU=6&amp;PvdD=5</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10&amp;CU=6&amp;PvdD=5&amp;FvD=5</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -9812,7 +9825,7 @@
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10&amp;CU=6&amp;PvdD=5&amp;FvD=5&amp;SGP=3</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -9820,11 +9833,11 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10&amp;CU=6&amp;PvdD=5&amp;FvD=5&amp;SGP=3&amp;Volt=3</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -9832,23 +9845,23 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10&amp;CU=6&amp;PvdD=5&amp;FvD=5&amp;SGP=3&amp;Volt=3&amp;DENK=2</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10&amp;CU=6&amp;PvdD=5&amp;FvD=5&amp;SGP=3&amp;Volt=3&amp;DENK=2&amp;JA21=2</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2&amp;CU=1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -9856,11 +9869,11 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10&amp;CU=6&amp;PvdD=5&amp;FvD=5&amp;SGP=3&amp;Volt=3&amp;DENK=2&amp;JA21=2&amp;50Plus=1</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2&amp;CU=1&amp;50plus=1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -9872,13 +9885,175 @@
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;PVV=19&amp;D66=18&amp;CDA=17&amp;PvdA=12&amp;SP=11&amp;GL=10&amp;CU=6&amp;PvdD=5&amp;FvD=5&amp;SGP=3&amp;Volt=3&amp;DENK=2&amp;JA21=2&amp;50Plus=1&amp;BBB=1</v>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2&amp;CU=1&amp;50plus=1&amp;BBB=1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2&amp;CU=1&amp;50plus=1&amp;BBB=1&amp;Bij1=1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="12">
+        <v>0.88541666666666663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>35</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>27</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B17">
-    <sortCondition descending="1" ref="A2"/>
+  <sortState ref="A44:B60">
+    <sortCondition descending="1" ref="A44"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tweede Kamerverkiezingen 98% geteld
</commit_message>
<xml_diff>
--- a/doc/tk.xlsx
+++ b/doc/tk.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="78">
   <si>
     <t>      Naam partij      </t>
   </si>
@@ -378,6 +378,9 @@
   <si>
     <t>exitpol</t>
   </si>
+  <si>
+    <t>98% geteld</t>
+  </si>
 </sst>
 </file>
 
@@ -494,7 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -528,6 +531,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9542,9 +9546,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -9564,35 +9568,35 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>17</v>
+      <c r="A3" s="13">
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -9600,28 +9604,28 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -9629,50 +9633,50 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -9709,15 +9713,15 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>27</v>
+      <c r="A23" s="13">
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>50</v>
       </c>
       <c r="C23" t="str">
         <f>C22&amp;"&amp;"&amp;B23&amp;"="&amp;A23</f>
-        <v>VVD=35&amp;D66=27</v>
+        <v>VVD=35&amp;D66=24</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -9729,19 +9733,19 @@
       </c>
       <c r="C24" t="str">
         <f t="shared" ref="C24:C38" si="0">C23&amp;"&amp;"&amp;B24&amp;"="&amp;A24</f>
-        <v>VVD=35&amp;D66=27&amp;PVV=17</v>
+        <v>VVD=35&amp;D66=24&amp;PVV=17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14</v>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -9749,23 +9753,23 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9</v>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8</v>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -9773,11 +9777,11 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8</v>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -9785,11 +9789,11 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7</v>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -9801,70 +9805,70 @@
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6</v>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7&amp;PvdD=6</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4</v>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7&amp;PvdD=6&amp;CU=5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7&amp;PvdD=6&amp;CU=5&amp;JA21=4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
         <v>8</v>
       </c>
-      <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>3</v>
-      </c>
-      <c r="B33" t="s">
-        <v>70</v>
-      </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7&amp;PvdD=6&amp;CU=5&amp;JA21=4&amp;SGP=3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7&amp;PvdD=6&amp;CU=5&amp;JA21=4&amp;SGP=3&amp;Volt=3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
         <v>75</v>
       </c>
-      <c r="C34" t="str">
-        <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35" t="s">
-        <v>66</v>
-      </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2&amp;CU=1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7&amp;PvdD=6&amp;CU=5&amp;JA21=4&amp;SGP=3&amp;Volt=3&amp;Denk=2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -9873,47 +9877,51 @@
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2&amp;CU=1&amp;50plus=1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7&amp;PvdD=6&amp;CU=5&amp;JA21=4&amp;SGP=3&amp;Volt=3&amp;Denk=2&amp;50plus=1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7&amp;PvdD=6&amp;CU=5&amp;JA21=4&amp;SGP=3&amp;Volt=3&amp;Denk=2&amp;50plus=1&amp;Bij1=1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="C37" t="str">
-        <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2&amp;CU=1&amp;50plus=1&amp;BBB=1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>73</v>
-      </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
-        <v>VVD=35&amp;D66=27&amp;PVV=17&amp;CDA=14&amp;PvdA=9&amp;GL=8&amp;SP=8&amp;FvD=7&amp;PvdD=6&amp;Volt=4&amp;SGP=3&amp;JA21=3&amp;Denk=2&amp;CU=1&amp;50plus=1&amp;BBB=1&amp;Bij1=1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>VVD=35&amp;D66=24&amp;PVV=17&amp;CDA=15&amp;SP=9&amp;PvdA=9&amp;FvD=8&amp;GL=7&amp;PvdD=6&amp;CU=5&amp;JA21=4&amp;SGP=3&amp;Volt=3&amp;Denk=2&amp;50plus=1&amp;Bij1=1&amp;BBB=1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>76</v>
       </c>
       <c r="C42" s="12">
         <v>0.88541666666666663</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <f>SUM(A44:A60)</f>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2021</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>35</v>
       </c>
@@ -9921,7 +9929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>27</v>
       </c>
@@ -9929,7 +9937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>17</v>
       </c>
@@ -9937,7 +9945,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>14</v>
       </c>
@@ -9945,7 +9953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9</v>
       </c>
@@ -9953,7 +9961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>8</v>
       </c>
@@ -9961,7 +9969,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>8</v>
       </c>
@@ -9969,7 +9977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7</v>
       </c>
@@ -9977,7 +9985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6</v>
       </c>
@@ -9985,7 +9993,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4</v>
       </c>
@@ -9993,7 +10001,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
@@ -10001,7 +10009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -10009,7 +10017,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2</v>
       </c>
@@ -10017,7 +10025,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1</v>
       </c>
@@ -10025,7 +10033,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1</v>
       </c>
@@ -10033,7 +10041,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -10041,7 +10049,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -10049,9 +10057,308 @@
         <v>73</v>
       </c>
     </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="12">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="D63">
+        <f>SUM(A65:A81)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>35</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>18</v>
+      </c>
+      <c r="B66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>14</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="13">
+        <v>26</v>
+      </c>
+      <c r="B68" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>8</v>
+      </c>
+      <c r="B70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>9</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>4</v>
+      </c>
+      <c r="B72" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>8</v>
+      </c>
+      <c r="B77" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>4</v>
+      </c>
+      <c r="B78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>35</v>
+      </c>
+      <c r="B86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="13">
+        <v>24</v>
+      </c>
+      <c r="B87" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>17</v>
+      </c>
+      <c r="B88" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>15</v>
+      </c>
+      <c r="B89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>9</v>
+      </c>
+      <c r="B90" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>9</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>8</v>
+      </c>
+      <c r="B92" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>7</v>
+      </c>
+      <c r="B93" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>6</v>
+      </c>
+      <c r="B94" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>5</v>
+      </c>
+      <c r="B95" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>4</v>
+      </c>
+      <c r="B96" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>3</v>
+      </c>
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>3</v>
+      </c>
+      <c r="B98" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="B99" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="B100" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="B101" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="B102" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A44:B60">
-    <sortCondition descending="1" ref="A44"/>
+  <sortState ref="A86:B102">
+    <sortCondition descending="1" ref="A86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>